<commit_message>
add some sections on movement
</commit_message>
<xml_diff>
--- a/Summaries/Paper + Book Summaries.xlsx
+++ b/Summaries/Paper + Book Summaries.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/Comprehensive-Exam-Notes/Summaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814C33D4-0904-C847-AD6A-9815410AE58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43563994-1E9C-DF48-A438-494D1EAD34B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scaling Fisheries" sheetId="1" r:id="rId1"/>
     <sheet name="Groundfish Biol + Ecol Papers" sheetId="2" r:id="rId2"/>
-    <sheet name="Growth Papers" sheetId="3" r:id="rId3"/>
-    <sheet name="Selectivity Papers" sheetId="4" r:id="rId4"/>
-    <sheet name="Composition Data Papers" sheetId="5" r:id="rId5"/>
-    <sheet name="Spatial Papers" sheetId="6" r:id="rId6"/>
-    <sheet name="Harvest + Reference Pt Papers" sheetId="7" r:id="rId7"/>
+    <sheet name="Pcod Stock Structure" sheetId="3" r:id="rId3"/>
+    <sheet name="Spatial Modelling" sheetId="6" r:id="rId4"/>
+    <sheet name="HCR" sheetId="7" r:id="rId5"/>
+    <sheet name="Reference Points" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="160">
   <si>
     <t>Section</t>
   </si>
@@ -1212,12 +1211,60 @@
 '- Sex-ratios can change - especially at the inital ages as well (i think shown for herring or capelin in Newfoundland). More work needs to be done to icnorparote these effects in that area. 
 '- Given changes in length-at-age, fecundity at age and length likely also changes simultaneously - more conservative measures of reference points might be neded given recent high recruitment events and prevailing environmental conditions.</t>
   </si>
+  <si>
+    <t>Spies et al. (2022) Genomic differentiation in Pacific cod using Pool-Seq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevance </t>
+  </si>
+  <si>
+    <t>- To look a genomic differnetation on a population genomics scale among EBS, AI, and WA spawning populations in Pcod, and identify drivers of differentiation</t>
+  </si>
+  <si>
+    <t>- Used Pool-Seq and a bunch of genetic techinques that I'm not all too faimilar with. 
+'- Also used Fst and absolute divergence indicators to detect whether there was genetic differentiation at speciefic locations of the genome. Fst = relative divergence could be due to lower within group genetic variation rather than divergence - whereas divergence is better measured with absolute divergence.
+'- Annotated parts of the genome to understand what genes they were differntiated and the function of those genes. 
+'- Correlated some of the Fst metrics against envrionmetanl covariates (temperature, salinity, veloctiy and chlorophyl). 
+'- Compared regions of the genome against EBS and AI, and EBS against WA. 
+'- Evaluated optical water detph (light penetration) between AI and EBS, because there the genomic regions identified were often assoicated with vision.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Regions of differentiation along the genome that are significant are called islands of divergence - this can be indicative of local adaptation for a species like Pcod that are in proximate locations. 
+'- These islands of differnetiation can arise due to hitchhiking, background selection, and chromosomal rearragenements (background selection = removal of deletious traits, hitchiking = impacted region impacts other linked regions, and chromsomal rearrangements = inversions). 
+'- Islands of differentatiation can also arise due to very strong selection processes - this process is often a tradeoff between migration-selection, wherein if the local adaptation and selection is stronger, the effects of gene flow are less important. 
+'- Selection and local adaptation in connected populations are important to understand because these populations are managed as their own populations units (i.e., stock structure). 
+'- Pacific cod exhibit isolation by distance selection, and there is thought to be 3 groups: 1) EBS, 2) AI, and 3) GOA. The GOA group is potenitally further differentiated into the eastern and western GOA subpopulations. 
+'- Adatpative divergence and genetic differentiation between the EBS and AI is likely due to differences in environment. In the EBS, it's more driven by ice extent dynamics, where the species compositions are often due to this, whereas in the AI, its more driven by currents, velocities, and passes altering the species composition there as well as light levels. This can lead to Pcod populations being more locally adpated to these condtions and feeding on these areas (e.g., Pcod in AI = more Atka mackerel, in EBS = more pollock). 
+'- In the AI, there is a strong abrupt shift in physical environment - west of Samalga Pass, there is warm nutrient water from the AK Coastal current, whereas in the east has more nutritent rich cold water.
+'- The southern populations of Pacific cod seem to be more related to Atlatnic cod due to divergence from the formation of the Bering Land Bridge.
+'- Recruitment and flow are important factors in Pacific cod recruitment, which could be a factor resulting in genetic differentiation between AI and EBS.
+'- Pools of the population generally differenitated based on lognitude - groups in the AI were more clustered with each other than Bering Sea, and there was distinct differnitaiton between the AK stocks and the WA stock. 
+'- Several regions of islands of differentiation were dtected between the EBS, AI, and WA, where Fst was way higher for allopatric populations - unsurprisingly. 
+'- The differentiation in some of the linkage regions were attributed to differentiation in vision related genes. 
+'- In the EBS and AI comparisons, the most significant correlates along some of the linkage groups were due to differences in velcotity and salinity. For EBS vs AI, this was salinity, velocity, chlorophyll, and then temperature.
+'-  The differentiation in vision related genes could be due to changes in light penetration - light penetration is way lower for the EBS than in the AI especially at 70m, and there is also some light breakage along Samalga Pass (darker in east than west). 
+'- The limited number of islands of divergence suggest a migration-selection balance, wherein the selection for traits for local adaptation are actually greater than gene flow (it does happen), resulting in divergence in those regions. (high Fst and elevated aboslute divergence). 
+'- There was high divergence between EBS and WA, but not EBS and AI along some distinct regions, consistent with the theory that gene flow acts to homogenize allele frequency except for regions greatly impacted by selection. 
+'- The islands of divergence in EBS-AI were also detected in EBS-WA suggesting that the visual genes are improtant for cod in terms of selection. 
+'- Correlates of velocity and salinty with regions of divergence related to vision are not surprising and these visual genes have been found to improtant for Atlantic cod. The selection for these genes are likley due to local adaptation wherien the EBS is darker than the AI. Also can be due to a geographic break along Samalga Pass where the east is dominated by chlorphyll coastal water whereas the west is more coastla nutrient clear rich water. Nonetheless, there appears to be some low level of gene flow among these populations. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Pacific cod exhibit stock structure between BS, AI, eastern GOA, and western GOA, and WA.
+'- Some of these differences appear to be attributed to geogrpahic reasons as well as currents. Namely the islands of diffferentiation were related to vision and EBS tends to be darker more driven by ice dynamics, while AI is genearlly more clear although with some influence of currents and passes. (east of Samalga Pass is darked with more chlorphyll mixed water comapred to the west).
+'- Recuritment of Pacific cod in the Bering sea has been shown to be related to velocity - velocity was found to be a key correalte in some of the regions of differneitation as well as salinity. However, temperature was less so. 
+'- Pacific cod exhibit an isolation-by-distance differentitation. Furthermore, the EBS and AI stocks appear to have some low levels of gene flow, but the migration-selection balance is great in terms of local adaptation. There is likely some gene flow between the two populations because the allele frequencies were similar across most regions between EBS-AI except for some regions (islands), whereas the allele frequencies were almost 2x that when comparing EBS-WA. That is to say, they are similar enough that there is likely gene flow going on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Pacific cod are separate stocks between EBS, AI, western GOA, and eastern GOA. 
+'- The regions of genomic differnetiaton appear to be related to vision, which could be due to geogrpahic features of these respective areas (EBS = darker, AI = lighter). 
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1270,6 +1317,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1312,7 +1366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1346,6 +1400,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1787,9 +1850,9 @@
   </sheetPr>
   <dimension ref="A1:Y999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -29011,45 +29074,42 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="1" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="65.1640625" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" customWidth="1"/>
-    <col min="7" max="7" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
+      <c r="F1" s="7" t="s">
+        <v>154</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -29068,7 +29128,26 @@
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A2" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29076,143 +29155,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" customWidth="1"/>
-    <col min="6" max="6" width="36.5" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -29280,7 +29222,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -29346,4 +29288,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92F4912-4F2B-9D4D-8EF1-23A5C054466B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:Z3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>